<commit_message>
agregar carga de remuneraciones y recaudaciones
se agregaron los modulos de carga de recaudaciones y remuneraciones. el modulo de remuneraciones solo permite carga a traves de importacion. el modulo de recaudaciones permite carga manual y a traves de importacion
</commit_message>
<xml_diff>
--- a/src/assets/plantillas/plantilla_gastos.xlsx
+++ b/src/assets/plantillas/plantilla_gastos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVIF\INFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7AFF3A-05C2-465C-9E84-53C49F0323BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6889506-A1C3-4210-B792-E89C2B5FC36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{775F9D82-D756-4AA9-9C4D-E0E8A7985217}"/>
   </bookViews>
@@ -18,7 +18,20 @@
   <definedNames>
     <definedName name="DatosExternos_1" localSheetId="0" hidden="1">plantilla_gastos!$A$1:$C$129</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -31,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="132">
   <si>
     <t>codigo_partida</t>
   </si>
@@ -936,15 +949,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -994,6 +1008,13 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
@@ -1008,13 +1029,6 @@
         <horizontal/>
       </border>
       <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1062,7 +1076,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C57BB382-082B-4341-B687-CEFCD10FCBBE}" uniqueName="1" name="codigo_partida" queryTableFieldId="1" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{45015BC3-CB4F-47F8-8820-2606B970FE83}" uniqueName="2" name="descripcion" queryTableFieldId="2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{E3624320-0512-46FC-B3E7-6F128E4406FA}" uniqueName="3" name="importe_devengado" queryTableFieldId="3" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{E3624320-0512-46FC-B3E7-6F128E4406FA}" uniqueName="3" name="importe_devengado" queryTableFieldId="3" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1387,8 +1401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B1F04CE-D35E-4589-ADCD-ADB9D2A57B77}">
   <dimension ref="A1:C129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E127" sqref="E127"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1416,7 +1430,6 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3">
@@ -1425,7 +1438,7 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1436,7 +1449,7 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5">
@@ -1445,9 +1458,7 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6">
@@ -1456,9 +1467,7 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7">
@@ -1467,7 +1476,7 @@
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1478,7 +1487,7 @@
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1489,7 +1498,7 @@
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1500,7 +1509,7 @@
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1511,7 +1520,7 @@
       <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1522,7 +1531,7 @@
       <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1533,7 +1542,7 @@
       <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1544,7 +1553,7 @@
       <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1555,7 +1564,7 @@
       <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1566,7 +1575,7 @@
       <c r="B16" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1577,7 +1586,7 @@
       <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1588,7 +1597,7 @@
       <c r="B18" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1599,7 +1608,7 @@
       <c r="B19" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1610,7 +1619,7 @@
       <c r="B20" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1621,7 +1630,7 @@
       <c r="B21" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1632,7 +1641,7 @@
       <c r="B22" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1643,7 +1652,7 @@
       <c r="B23" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1654,7 +1663,7 @@
       <c r="B24" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1665,9 +1674,7 @@
       <c r="B25" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26">
@@ -1676,7 +1683,7 @@
       <c r="B26" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1687,7 +1694,7 @@
       <c r="B27" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1698,7 +1705,7 @@
       <c r="B28" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1709,7 +1716,7 @@
       <c r="B29" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1720,7 +1727,7 @@
       <c r="B30" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1731,7 +1738,7 @@
       <c r="B31" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1742,7 +1749,7 @@
       <c r="B32" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1753,7 +1760,7 @@
       <c r="B33" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1764,7 +1771,7 @@
       <c r="B34" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1775,7 +1782,7 @@
       <c r="B35" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1786,7 +1793,7 @@
       <c r="B36" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1797,7 +1804,7 @@
       <c r="B37" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1808,7 +1815,7 @@
       <c r="B38" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1819,7 +1826,7 @@
       <c r="B39" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1830,7 +1837,7 @@
       <c r="B40" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1841,7 +1848,7 @@
       <c r="B41" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1852,7 +1859,7 @@
       <c r="B42" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1863,7 +1870,7 @@
       <c r="B43" t="s">
         <v>45</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1874,7 +1881,7 @@
       <c r="B44" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1885,7 +1892,7 @@
       <c r="B45" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1896,7 +1903,7 @@
       <c r="B46" t="s">
         <v>48</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1907,7 +1914,7 @@
       <c r="B47" t="s">
         <v>49</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1918,7 +1925,7 @@
       <c r="B48" t="s">
         <v>50</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1929,7 +1936,7 @@
       <c r="B49" t="s">
         <v>51</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1940,7 +1947,7 @@
       <c r="B50" t="s">
         <v>52</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1951,7 +1958,7 @@
       <c r="B51" t="s">
         <v>53</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1962,7 +1969,7 @@
       <c r="B52" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1973,7 +1980,7 @@
       <c r="B53" t="s">
         <v>55</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1984,7 +1991,7 @@
       <c r="B54" t="s">
         <v>56</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1995,7 +2002,7 @@
       <c r="B55" t="s">
         <v>57</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2006,7 +2013,7 @@
       <c r="B56" t="s">
         <v>58</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2017,7 +2024,7 @@
       <c r="B57" t="s">
         <v>59</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2028,7 +2035,7 @@
       <c r="B58" t="s">
         <v>60</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2039,7 +2046,7 @@
       <c r="B59" t="s">
         <v>61</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2050,7 +2057,7 @@
       <c r="B60" t="s">
         <v>62</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2061,7 +2068,7 @@
       <c r="B61" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2072,7 +2079,7 @@
       <c r="B62" t="s">
         <v>64</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2083,7 +2090,7 @@
       <c r="B63" t="s">
         <v>65</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2094,7 +2101,7 @@
       <c r="B64" t="s">
         <v>66</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2105,7 +2112,7 @@
       <c r="B65" t="s">
         <v>67</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2116,7 +2123,7 @@
       <c r="B66" t="s">
         <v>74</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2127,7 +2134,7 @@
       <c r="B67" t="s">
         <v>75</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C67" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2138,7 +2145,7 @@
       <c r="B68" t="s">
         <v>76</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2149,7 +2156,7 @@
       <c r="B69" t="s">
         <v>77</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C69" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2160,7 +2167,7 @@
       <c r="B70" t="s">
         <v>78</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2171,7 +2178,7 @@
       <c r="B71" t="s">
         <v>79</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C71" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2182,7 +2189,7 @@
       <c r="B72" t="s">
         <v>80</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C72" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2193,7 +2200,7 @@
       <c r="B73" t="s">
         <v>81</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C73" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2204,7 +2211,7 @@
       <c r="B74" t="s">
         <v>82</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2215,7 +2222,7 @@
       <c r="B75" t="s">
         <v>68</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C75" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2226,7 +2233,7 @@
       <c r="B76" t="s">
         <v>83</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2237,7 +2244,7 @@
       <c r="B77" t="s">
         <v>84</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C77" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2248,7 +2255,7 @@
       <c r="B78" t="s">
         <v>85</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2259,7 +2266,7 @@
       <c r="B79" t="s">
         <v>86</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2270,7 +2277,7 @@
       <c r="B80" t="s">
         <v>87</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C80" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2281,7 +2288,7 @@
       <c r="B81" t="s">
         <v>88</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2292,7 +2299,7 @@
       <c r="B82" t="s">
         <v>89</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C82" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2303,7 +2310,7 @@
       <c r="B83" t="s">
         <v>90</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C83" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2314,7 +2321,7 @@
       <c r="B84" t="s">
         <v>91</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C84" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2325,7 +2332,7 @@
       <c r="B85" t="s">
         <v>69</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C85" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2336,7 +2343,7 @@
       <c r="B86" t="s">
         <v>92</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C86" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2347,7 +2354,7 @@
       <c r="B87" t="s">
         <v>93</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C87" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2358,7 +2365,7 @@
       <c r="B88" t="s">
         <v>94</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C88" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2369,7 +2376,7 @@
       <c r="B89" t="s">
         <v>95</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C89" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2380,7 +2387,7 @@
       <c r="B90" t="s">
         <v>96</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2391,7 +2398,7 @@
       <c r="B91" t="s">
         <v>97</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C91" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2402,7 +2409,7 @@
       <c r="B92" t="s">
         <v>98</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C92" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2413,7 +2420,7 @@
       <c r="B93" t="s">
         <v>99</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C93" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2424,7 +2431,7 @@
       <c r="B94" t="s">
         <v>100</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C94" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2435,7 +2442,7 @@
       <c r="B95" t="s">
         <v>70</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="C95" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2446,7 +2453,7 @@
       <c r="B96" t="s">
         <v>101</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="C96" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2457,7 +2464,7 @@
       <c r="B97" t="s">
         <v>102</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C97" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2468,7 +2475,7 @@
       <c r="B98" t="s">
         <v>103</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="C98" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2479,7 +2486,7 @@
       <c r="B99" t="s">
         <v>104</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C99" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2490,7 +2497,7 @@
       <c r="B100" t="s">
         <v>105</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C100" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2501,7 +2508,7 @@
       <c r="B101" t="s">
         <v>106</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2512,7 +2519,7 @@
       <c r="B102" t="s">
         <v>107</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C102" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2523,7 +2530,7 @@
       <c r="B103" t="s">
         <v>108</v>
       </c>
-      <c r="C103" s="3" t="s">
+      <c r="C103" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2534,7 +2541,7 @@
       <c r="B104" t="s">
         <v>109</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="C104" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2545,7 +2552,7 @@
       <c r="B105" t="s">
         <v>71</v>
       </c>
-      <c r="C105" s="3" t="s">
+      <c r="C105" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2556,7 +2563,7 @@
       <c r="B106" t="s">
         <v>110</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="C106" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2567,7 +2574,7 @@
       <c r="B107" t="s">
         <v>111</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="C107" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2578,7 +2585,7 @@
       <c r="B108" t="s">
         <v>112</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="C108" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2589,7 +2596,7 @@
       <c r="B109" t="s">
         <v>113</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="C109" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2600,7 +2607,7 @@
       <c r="B110" t="s">
         <v>114</v>
       </c>
-      <c r="C110" s="2" t="s">
+      <c r="C110" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2611,7 +2618,7 @@
       <c r="B111" t="s">
         <v>115</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="C111" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2622,7 +2629,7 @@
       <c r="B112" t="s">
         <v>116</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C112" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2633,7 +2640,7 @@
       <c r="B113" t="s">
         <v>117</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="C113" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2644,7 +2651,7 @@
       <c r="B114" t="s">
         <v>72</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="C114" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2655,7 +2662,7 @@
       <c r="B115" t="s">
         <v>118</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C115" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2666,7 +2673,7 @@
       <c r="B116" t="s">
         <v>119</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="C116" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2677,7 +2684,7 @@
       <c r="B117" t="s">
         <v>120</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C117" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2688,7 +2695,7 @@
       <c r="B118" t="s">
         <v>121</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="C118" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2699,7 +2706,7 @@
       <c r="B119" t="s">
         <v>122</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C119" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2710,7 +2717,7 @@
       <c r="B120" t="s">
         <v>123</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="C120" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2721,7 +2728,7 @@
       <c r="B121" t="s">
         <v>124</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="C121" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2732,7 +2739,7 @@
       <c r="B122" t="s">
         <v>125</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C122" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2743,7 +2750,7 @@
       <c r="B123" t="s">
         <v>126</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="C123" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2754,7 +2761,7 @@
       <c r="B124" t="s">
         <v>73</v>
       </c>
-      <c r="C124" s="3"/>
+      <c r="C124" s="2"/>
     </row>
     <row r="125" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A125">
@@ -2763,7 +2770,7 @@
       <c r="B125" t="s">
         <v>127</v>
       </c>
-      <c r="C125" s="2" t="s">
+      <c r="C125" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2774,7 +2781,7 @@
       <c r="B126" t="s">
         <v>128</v>
       </c>
-      <c r="C126" s="2" t="s">
+      <c r="C126" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2785,7 +2792,7 @@
       <c r="B127" t="s">
         <v>129</v>
       </c>
-      <c r="C127" s="2" t="s">
+      <c r="C127" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2796,7 +2803,7 @@
       <c r="B128" t="s">
         <v>130</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="C128" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2807,14 +2814,14 @@
       <c r="B129" t="s">
         <v>131</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="C129" s="1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8w2QgXYRFg/wBPzmV4wvizhOD+loNssa3ZuyT5qIa0TWZptKe9d11FlWqexcNEP+gK9fptQvXMiE8c5aKrkauQ==" saltValue="sZYxicIcYDSc+/QO3/yTfw==" spinCount="100000" sheet="1" formatCells="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="PFfbVnHyqwmsMV/VnJZQXCO4x8dPvgjcFGta3bHGUy9vAeeuCABomKhPauxoTr9c7OHALhmmfyr+ct4Y+UQcAA==" saltValue="3KCpeaYLR9l/HJUhR6Z8cw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <conditionalFormatting sqref="A2:C129">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>NOT(ISERROR(SEARCH("(NO CARGAR)",$B2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>